<commit_message>
ReadBook Service - Naver API
</commit_message>
<xml_diff>
--- a/SpMVC_Readbook/독서록프로젝트 테이블명세.xlsx
+++ b/SpMVC_Readbook/독서록프로젝트 테이블명세.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>열 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -107,6 +107,180 @@
   </si>
   <si>
     <t>신민석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>pubdate</t>
+  </si>
+  <si>
+    <t>문자열(125)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열(255)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열(2000)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열(15)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도서명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세정보링크</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도서이미지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>할인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>출판사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>출판일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구입일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열(10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구입가격</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구입처</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>buydate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>buyprice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>buystore</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nVARCHAR2(125)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nVARCHAR2(255)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nVARCHAR2(125)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR(13)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nVARCHAR2(2000)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR(15)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR(10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nVARCHAR2(50)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>일련번호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seq</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRIMARY KEY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT NULL</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -117,7 +291,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -150,6 +324,13 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -171,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -372,13 +553,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -470,6 +724,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -816,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:L3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1566,12 +1841,22 @@
       <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>61</v>
+      </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1581,11 +1866,21 @@
       <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="C6" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1596,10 +1891,18 @@
       <c r="B7" s="10">
         <v>3</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="4"/>
+      <c r="C7" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="G7" s="14"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1611,10 +1914,18 @@
       <c r="B8" s="10">
         <v>4</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="4"/>
+      <c r="C8" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1626,10 +1937,18 @@
       <c r="B9" s="10">
         <v>5</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="4"/>
+      <c r="C9" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="G9" s="14"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -1641,10 +1960,18 @@
       <c r="B10" s="10">
         <v>6</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="4"/>
+      <c r="C10" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1656,10 +1983,18 @@
       <c r="B11" s="10">
         <v>7</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="C11" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G11" s="14"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1671,10 +2006,18 @@
       <c r="B12" s="10">
         <v>8</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="4"/>
+      <c r="C12" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1686,10 +2029,18 @@
       <c r="B13" s="10">
         <v>9</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="4"/>
+      <c r="C13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1701,10 +2052,18 @@
       <c r="B14" s="10">
         <v>10</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="4"/>
+      <c r="C14" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1716,10 +2075,18 @@
       <c r="B15" s="10">
         <v>11</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="4"/>
+      <c r="C15" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1731,10 +2098,18 @@
       <c r="B16" s="10">
         <v>12</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="4"/>
+      <c r="C16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1746,10 +2121,18 @@
       <c r="B17" s="10">
         <v>13</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1761,10 +2144,18 @@
       <c r="B18" s="10">
         <v>14</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1776,10 +2167,10 @@
       <c r="B19" s="10">
         <v>15</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -1791,10 +2182,10 @@
       <c r="B20" s="12">
         <v>16</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>

</xml_diff>